<commit_message>
feat: now it generates vehicle columns
</commit_message>
<xml_diff>
--- a/output/Planilha_Contagem.xlsx
+++ b/output/Planilha_Contagem.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,6 +33,9 @@
       <b val="1"/>
       <color rgb="00FF0000"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -49,7 +52,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -63,17 +66,29 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -462,7 +477,7 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
-          <t>P001</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -559,7 +574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,34 +585,274 @@
     <col width="2" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="7" max="7"/>
+    <col width="5" customWidth="1" min="8" max="8"/>
+    <col width="11" customWidth="1" min="9" max="9"/>
+    <col width="9" customWidth="1" min="10" max="10"/>
+    <col width="9" customWidth="1" min="11" max="11"/>
+    <col width="9" customWidth="1" min="12" max="12"/>
+    <col width="5" customWidth="1" min="13" max="13"/>
+    <col width="5" customWidth="1" min="14" max="14"/>
+    <col width="5" customWidth="1" min="15" max="15"/>
+    <col width="5" customWidth="1" min="16" max="16"/>
+    <col width="5" customWidth="1" min="17" max="17"/>
+    <col width="5" customWidth="1" min="18" max="18"/>
+    <col width="8" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="7" customWidth="1" min="21" max="21"/>
+    <col width="9" customWidth="1" min="22" max="22"/>
+    <col width="11" customWidth="1" min="23" max="23"/>
+    <col width="8" customWidth="1" min="24" max="24"/>
+    <col width="10" customWidth="1" min="25" max="25"/>
+    <col width="8" customWidth="1" min="26" max="26"/>
+    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="7" customWidth="1" min="28" max="28"/>
+    <col width="7" customWidth="1" min="29" max="29"/>
+    <col width="17" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Data:</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>04-05-2025</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>Movimento:</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>04-05-2025</t>
+          <t>1A</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Movimentos</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>P001A</t>
-        </is>
-      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Horas</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Leves</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>Carretinha</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>VUC</t>
+        </is>
+      </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>Caminhões</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="n"/>
+      <c r="K3" s="4" t="n"/>
+      <c r="L3" s="4" t="inlineStr">
+        <is>
+          <t>Carreta</t>
+        </is>
+      </c>
+      <c r="M3" s="4" t="n"/>
+      <c r="N3" s="4" t="n"/>
+      <c r="O3" s="4" t="n"/>
+      <c r="P3" s="4" t="n"/>
+      <c r="Q3" s="4" t="n"/>
+      <c r="R3" s="4" t="n"/>
+      <c r="S3" s="4" t="inlineStr">
+        <is>
+          <t>Ônibus</t>
+        </is>
+      </c>
+      <c r="T3" s="4" t="n"/>
+      <c r="U3" s="4" t="inlineStr">
+        <is>
+          <t>Motos</t>
+        </is>
+      </c>
+      <c r="V3" s="4" t="inlineStr">
+        <is>
+          <t>Pesados</t>
+        </is>
+      </c>
+      <c r="W3" s="4" t="n"/>
+      <c r="X3" s="4" t="n"/>
+      <c r="Y3" s="4" t="n"/>
+      <c r="Z3" s="4" t="n"/>
+      <c r="AA3" s="4" t="n"/>
+      <c r="AB3" s="4" t="n"/>
+      <c r="AC3" s="4" t="n"/>
+      <c r="AD3" s="4" t="inlineStr">
+        <is>
+          <t>Veículos Totais</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>as</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n"/>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>1 Eixo</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>2 Eixos</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>3 Eixos</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="n"/>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>2 Eixos</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>3 Eixos</t>
+        </is>
+      </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>4 Eixos</t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>2 E</t>
+        </is>
+      </c>
+      <c r="M4" s="5" t="inlineStr">
+        <is>
+          <t>3 E</t>
+        </is>
+      </c>
+      <c r="N4" s="5" t="inlineStr">
+        <is>
+          <t>4 E</t>
+        </is>
+      </c>
+      <c r="O4" s="5" t="inlineStr">
+        <is>
+          <t>5 E</t>
+        </is>
+      </c>
+      <c r="P4" s="5" t="inlineStr">
+        <is>
+          <t>6 E</t>
+        </is>
+      </c>
+      <c r="Q4" s="5" t="inlineStr">
+        <is>
+          <t>7 E</t>
+        </is>
+      </c>
+      <c r="R4" s="5" t="inlineStr">
+        <is>
+          <t>8 E</t>
+        </is>
+      </c>
+      <c r="S4" s="5" t="inlineStr">
+        <is>
+          <t>2 E</t>
+        </is>
+      </c>
+      <c r="T4" s="5" t="inlineStr">
+        <is>
+          <t>3 E ou +</t>
+        </is>
+      </c>
+      <c r="U4" s="4" t="n"/>
+      <c r="V4" s="5" t="inlineStr">
+        <is>
+          <t>% Cam</t>
+        </is>
+      </c>
+      <c r="W4" s="5" t="inlineStr">
+        <is>
+          <t>Caminhões</t>
+        </is>
+      </c>
+      <c r="X4" s="5" t="inlineStr">
+        <is>
+          <t>% Carr</t>
+        </is>
+      </c>
+      <c r="Y4" s="5" t="inlineStr">
+        <is>
+          <t>Carretas</t>
+        </is>
+      </c>
+      <c r="Z4" s="5" t="inlineStr">
+        <is>
+          <t>% Ônib</t>
+        </is>
+      </c>
+      <c r="AA4" s="5" t="inlineStr">
+        <is>
+          <t>Ônibus</t>
+        </is>
+      </c>
+      <c r="AB4" s="5" t="inlineStr">
+        <is>
+          <t>% Pes</t>
+        </is>
+      </c>
+      <c r="AC4" s="5" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="AD4" s="4" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="V3:AC3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:R3"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S3:T3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>